<commit_message>
2nd Scenario sample for ASYNC done
</commit_message>
<xml_diff>
--- a/Parallel_Programming/Scenarios_To_Consider_While_Studying_Parallel_Programming.xlsx
+++ b/Parallel_Programming/Scenarios_To_Consider_While_Studying_Parallel_Programming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\git\all-languages\Parallel_Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293826BD-781C-459D-8A80-6042585E55B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AE7D2B-98FC-4F75-8C64-C077FA4D1A09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Performing long running tasks/heavy computation task on another thread without blocking UI</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>long running tasks/heavy computation task - blocks UI</t>
+  </si>
+  <si>
+    <t>ASYNC</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -364,39 +370,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="78.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Scenario 3 Exception Occurs in another thread
</commit_message>
<xml_diff>
--- a/Parallel_Programming/Scenarios_To_Consider_While_Studying_Parallel_Programming.xlsx
+++ b/Parallel_Programming/Scenarios_To_Consider_While_Studying_Parallel_Programming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\git\all-languages\Parallel_Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AE7D2B-98FC-4F75-8C64-C077FA4D1A09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94EA6FA-B334-46C0-83EC-EAA7AEBA3FFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Performing long running tasks/heavy computation task on another thread without blocking UI</t>
   </si>
@@ -87,9 +87,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,7 +376,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -400,12 +403,16 @@
       <c r="B4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" t="s">
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" t="s">
         <v>1</v>
       </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
@@ -420,6 +427,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C4:C5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>